<commit_message>
DTP for Exit to MainMenu
DTP for Exit to MainMenu via ESC Key
</commit_message>
<xml_diff>
--- a/Documents/Software/Testing and Integration/eCook's DTP Record - GraphicsHandler.xlsx
+++ b/Documents/Software/Testing and Integration/eCook's DTP Record - GraphicsHandler.xlsx
@@ -745,9 +745,6 @@
     <t>Only exit fullscreemode. Does not return to Main Menu</t>
   </si>
   <si>
-    <t>Only one videos play as one of the http does not work.(Based on Playlist 2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Video/Audio still continues to play. </t>
   </si>
   <si>
@@ -758,6 +755,9 @@
   </si>
   <si>
     <t>Resets to 00:00:00</t>
+  </si>
+  <si>
+    <t>Only one of the videos plays as one of the http does not work.(Based on Playlist 2)</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1205,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1215,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2117,7 @@
         <v>114</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2386,7 +2386,7 @@
         <v>114</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -2940,7 +2940,7 @@
         <v>113</v>
       </c>
       <c r="F112" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G112" s="25"/>
       <c r="H112" s="25"/>
@@ -2979,7 +2979,7 @@
         <v>114</v>
       </c>
       <c r="F113" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G113" s="25"/>
       <c r="H113" s="25"/>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="115" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A115" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>